<commit_message>
Added test-cases-16.04.2017.xlsx and additional requirements
</commit_message>
<xml_diff>
--- a/Team_Papaya_Tasks.xlsx
+++ b/Team_Papaya_Tasks.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Team Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -36,7 +44,7 @@
   <si>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="9"/>
         <color indexed="8"/>
         <rFont val="Tahoma"/>
@@ -76,7 +84,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="9"/>
         <color indexed="11"/>
         <rFont val="Tahoma"/>
@@ -86,9 +94,6 @@
   </si>
   <si>
     <t>Create a GitHub acconts and add to repository</t>
-  </si>
-  <si>
-    <t>in progress</t>
   </si>
   <si>
     <r>
@@ -119,9 +124,6 @@
     <t>Write a SRS document.</t>
   </si>
   <si>
-    <t>Write a Testplan for functionality test.</t>
-  </si>
-  <si>
     <t>Write test scenarios with test case</t>
   </si>
   <si>
@@ -159,45 +161,38 @@
   </si>
   <si>
     <t>Final Presentation of the project</t>
+  </si>
+  <si>
+    <t>hbahnev, PeUzunov</t>
+  </si>
+  <si>
+    <t>Write a Test plan for functionality test.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color indexed="8"/>
       <name val="Tahoma"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Tahoma"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="9"/>
       <color indexed="8"/>
       <name val="Tahoma"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="9"/>
       <color indexed="11"/>
       <name val="Tahoma"/>
@@ -272,44 +267,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -318,26 +297,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff0563c1"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF0563C1"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -539,7 +577,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -558,7 +596,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -588,7 +626,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -614,7 +652,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -640,7 +678,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -666,7 +704,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -692,7 +730,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -718,7 +756,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -744,7 +782,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -770,7 +808,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -796,7 +834,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -809,9 +847,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -828,7 +872,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -847,7 +891,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -873,7 +917,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -899,7 +943,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -925,7 +969,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -951,7 +995,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -977,7 +1021,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1003,7 +1047,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1029,7 +1073,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,7 +1099,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1081,7 +1125,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1094,9 +1138,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1110,7 +1160,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1129,7 +1179,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1159,7 +1209,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1185,7 +1235,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1211,7 +1261,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1237,7 +1287,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1263,7 +1313,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1289,7 +1339,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1315,7 +1365,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1341,7 +1391,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1367,7 +1417,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1380,423 +1430,436 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV39"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.21094" style="1" customWidth="1"/>
-    <col min="2" max="2" width="71.6016" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.8125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.8125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="80.1094" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="80.140625" style="1" customWidth="1"/>
     <col min="6" max="256" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1">
+    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="14" customHeight="1">
+    <row r="2" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="14" customHeight="1">
+    <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s" s="5">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" ht="14" customHeight="1">
+    <row r="4" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="5">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="6">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s" s="6">
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" ht="14" customHeight="1">
+    </row>
+    <row r="5" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s" s="6">
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="14" customHeight="1">
+    <row r="6" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="5">
-        <v>15</v>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" ht="14" customHeight="1">
+    <row r="7" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="5">
-        <v>16</v>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="14" customHeight="1">
+    <row r="8" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="5">
-        <v>17</v>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" ht="14" customHeight="1">
+    <row r="9" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="5">
-        <v>18</v>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" ht="14" customHeight="1">
+    <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7"/>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" ht="14" customHeight="1">
+      <c r="E10" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="5">
-        <v>20</v>
+      <c r="B11" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" ht="14" customHeight="1">
+    <row r="12" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="5">
-        <v>21</v>
+      <c r="B12" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" ht="14" customHeight="1">
+    <row r="13" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="5">
-        <v>22</v>
+      <c r="B13" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" ht="14" customHeight="1">
+    <row r="14" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="5">
-        <v>23</v>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" ht="14" customHeight="1">
+    <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="5">
-        <v>24</v>
+      <c r="B15" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" ht="14" customHeight="1">
+    <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="5">
-        <v>25</v>
+      <c r="B16" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" ht="14" customHeight="1">
+    <row r="17" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="5">
-        <v>26</v>
+      <c r="B17" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" ht="14" customHeight="1">
+    <row r="18" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" t="s" s="5">
-        <v>27</v>
+      <c r="B18" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" ht="14" customHeight="1">
+    <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="5">
-        <v>25</v>
+      <c r="B19" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" ht="14" customHeight="1">
+    <row r="20" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="5">
-        <v>28</v>
+      <c r="B20" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" ht="14" customHeight="1">
+    <row r="21" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="5">
-        <v>29</v>
+      <c r="B21" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" ht="14" customHeight="1">
+    <row r="22" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="5">
-        <v>30</v>
+      <c r="B22" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" ht="14" customHeight="1">
+    <row r="23" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" t="s" s="5">
-        <v>31</v>
+      <c r="B23" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" ht="14" customHeight="1">
+    <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" t="s" s="5">
-        <v>32</v>
+      <c r="B24" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" ht="14" customHeight="1">
+    <row r="25" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" t="s" s="5">
-        <v>33</v>
+      <c r="B25" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" ht="14" customHeight="1">
+    <row r="26" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" ht="14" customHeight="1">
+    <row r="27" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" ht="14" customHeight="1">
+    <row r="28" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="8"/>
       <c r="B28" s="10"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" ht="14" customHeight="1">
+    <row r="29" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" ht="14" customHeight="1">
+    <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" ht="14" customHeight="1">
+    <row r="31" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" ht="14" customHeight="1">
+    <row r="32" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" ht="14" customHeight="1">
+    <row r="33" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" ht="14" customHeight="1">
+    <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" ht="14" customHeight="1">
+    <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" ht="14" customHeight="1">
+    <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" ht="14" customHeight="1">
+    <row r="37" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" ht="14" customHeight="1">
+    <row r="38" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" ht="14" customHeight="1">
+    <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1805,10 +1868,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="E3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
just an empty commit
To test trigger
</commit_message>
<xml_diff>
--- a/Team_Papaya_Tasks.xlsx
+++ b/Team_Papaya_Tasks.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Team Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,10 +158,10 @@
     <t>Final Presentation of the project</t>
   </si>
   <si>
-    <t>hbahnev, PeUzunov</t>
-  </si>
-  <si>
     <t>Write a Test plan for functionality test.</t>
+  </si>
+  <si>
+    <t>hbahnev, PeUzunov,</t>
   </si>
 </sst>
 </file>
@@ -1452,7 +1447,7 @@
   <dimension ref="A1:IV39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1600,7 +1595,7 @@
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
@@ -1608,7 +1603,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>

</xml_diff>